<commit_message>
- Added link and pop-up buttons to the dashboard. Fixed a few minor bugs.
</commit_message>
<xml_diff>
--- a/www/definitions.xlsx
+++ b/www/definitions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Isdsf00d03\cl-out\MetadataCatalogue\dashboard_code\metadata-catalogue-dashboard\www\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\stats\cl-out\MetadataCatalogue\dashboard_code\metadata-catalogue-dashboard\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB73520-0ECD-4ED9-BADE-2A560D9C60C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EFF9CC1-152A-4BB1-9778-74719C8C9BB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6E15B39E-F836-4E17-87F3-3087AF82566E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6E15B39E-F836-4E17-87F3-3087AF82566E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="62">
   <si>
     <t>Definition</t>
   </si>
@@ -191,40 +191,37 @@
     <t>Should this ever be empty? Or should all items be labeled as either internal or external?</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
     <t>Should this ever be empty?</t>
   </si>
   <si>
     <t>Produced by PHS</t>
   </si>
   <si>
-    <t>Indicator, Dashboard, Statistical report</t>
-  </si>
-  <si>
-    <t>broken down by female &amp; male, female only, male only</t>
-  </si>
-  <si>
-    <t>Age, sex, SIMD, deprivation, religion, sexual orientation, income, long term conditions, urban/rural</t>
-  </si>
-  <si>
-    <t>Scotland, NHS Board, Treatment Centre, Intermediate zone, HSCP, Health board, Local Authority, Alcohol &amp; Drug Partnership, GP Practice,  GP Practice Cluster, Hospital, Prison</t>
-  </si>
-  <si>
     <t>A URL link or links to where the data item can be found.</t>
   </si>
   <si>
-    <t>1 yearly, 2 yearly, 3 yearly, 4 yearly, Adhoc, Monthly, Quarterly, Weekly</t>
-  </si>
-  <si>
-    <t>Health &amp; Care: Acute &amp; Emergency Services, Justice Crime &amp; Violence, Early Years &amp; Young People, Alcohol : Drugs : Smoking, Health &amp; Care: Primary Community &amp; Social Care, Education, Long Term Conditions &amp; Diseases, Place &amp; physical environment, Dental Health, Housing, Income &amp; Poverty, GCR Indicators, Mental health &amp; Wellbeing,  Communicable diseases, Physical Activity, Transport, Vulnerable Populations, Diet &amp; Nutrition, Employment, Vaccinations, Place &amp; Physical Environment,  Climate &amp; Environment,  Gambling, Children &amp; Young People, Tobacco</t>
-  </si>
-  <si>
-    <t>IVF, Hosital care, Crime, Alcohol, Children, Drugs, Social care, Mental health, Disease register, Participation, Acute care, Home care, ADHD, Dentist, Out of hours, Prescribing, Palliative care, Tobacco, Falls, Population health, Place, Multiple sclerosis, Weight, Asthma, Poverty, PPI, Cancer, Food, Active travel, Unpaid care, Life expectancy, Prison, Arthroplasty, Poisonings, Knee replacement, Suicide, Mucolytics, Employment, Pregnancy, Vaccinations, Healthcare audits, Anaesthetic, GP, Virus, Deaths, Injury, Climate change, Finance, Hernia, Surgery, Diabetes, CHD, Vaccinations, COPD, Crime, Physical activity, Trauma, Hip replacement, Technology, Chronic pain, Breastfeeding, CKD, Naloxone, COVID-19,  Injuries, Waiting times, Osteoporosis, Cardiovascular, Hypertension, Gambling, Dementia, Benefits, SHS, NRS</t>
-  </si>
-  <si>
     <t>Possible values</t>
+  </si>
+  <si>
+    <t>1 yearly| 2 yearly| 3 yearly| 4 yearly| Adhoc| Monthly| Quarterly| Weekly</t>
+  </si>
+  <si>
+    <t>Scotland| NHS Board| Treatment Centre| Intermediate zone| HSCP| Health board| Local Authority| Alcohol &amp; Drug Partnership| GP Practice|  GP Practice Cluster| Hospital| Prison</t>
+  </si>
+  <si>
+    <t>Age| sex| SIMD| deprivation| religion| sexual orientation| income| long term conditions| urban/rural</t>
+  </si>
+  <si>
+    <t>broken down by female &amp; male| female only| male only</t>
+  </si>
+  <si>
+    <t>Indicator| Dashboard| Statistical report</t>
+  </si>
+  <si>
+    <t>IVF| Hosital care| Crime| Alcohol| Children| Drugs| Social care| Mental health| Disease register| Participation| Acute care| Home care| ADHD| Dentist| Out of hours| Prescribing| Palliative care| Tobacco| Falls| Population health| Place| Multiple sclerosis| Weight| Asthma| Poverty| PPI| Cancer| Food| Active travel| Unpaid care| Life expectancy| Prison| Arthroplasty| Poisonings| Knee replacement| Suicide| Mucolytics| Employment| Pregnancy| Vaccinations| Healthcare audits| Anaesthetic| GP| Virus| Deaths| Injury| Climate change| Finance| Hernia| Surgery| Diabetes| CHD| Vaccinations| COPD| Crime| Physical activity| Trauma| Hip replacement| Technology| Chronic pain| Breastfeeding| CKD| Naloxone| COVID-19|  Injuries| Waiting times| Osteoporosis| Cardiovascular| Hypertension| Gambling| Dementia| Benefits| SHS| NRS</t>
+  </si>
+  <si>
+    <t>Health &amp; Care: Acute &amp; Emergency Services| Justice Crime &amp; Violence| Early Years &amp; Young People| Alcohol : Drugs : Smoking| Health &amp; Care: Primary Community &amp; Social Care| Education| Long Term Conditions &amp; Diseases| Place &amp; physical environment| Dental Health| Housing| Income &amp; Poverty| GCR Indicators| Mental health &amp; Wellbeing|  Communicable diseases| Physical Activity| Transport| Vulnerable Populations| Diet &amp; Nutrition| Employment| Vaccinations| Place &amp; Physical Environment|  Climate &amp; Environment|  Gambling| Children &amp; Young People| Tobacco</t>
   </si>
 </sst>
 </file>
@@ -628,20 +625,20 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.36328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.81640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="60.54296875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="71.1796875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="60.5703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="71.140625" style="2" customWidth="1"/>
     <col min="6" max="6" width="80" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
@@ -652,7 +649,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>38</v>
@@ -661,7 +658,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -673,7 +670,7 @@
       </c>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -690,7 +687,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="109" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="108.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -701,13 +698,13 @@
         <v>28</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="109" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="108.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -718,11 +715,11 @@
         <v>20</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -733,11 +730,11 @@
         <v>19</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -754,9 +751,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>40</v>
@@ -769,7 +766,7 @@
       </c>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -781,7 +778,7 @@
       </c>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -793,7 +790,7 @@
       </c>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" ht="116" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
@@ -810,7 +807,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
@@ -821,10 +818,10 @@
         <v>34</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -835,11 +832,11 @@
         <v>25</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -850,11 +847,11 @@
         <v>27</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -862,11 +859,11 @@
         <v>39</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
@@ -878,7 +875,7 @@
       </c>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>9</v>
       </c>
@@ -889,14 +886,14 @@
         <v>26</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -908,7 +905,7 @@
       </c>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>12</v>
       </c>
@@ -920,7 +917,7 @@
       </c>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>32</v>
       </c>
@@ -929,9 +926,6 @@
       </c>
       <c r="C20" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="F20" s="2"/>
     </row>

</xml_diff>

<commit_message>
- added accessible download excels - fixed several accessibility issues
</commit_message>
<xml_diff>
--- a/www/definitions.xlsx
+++ b/www/definitions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\stats\cl-out\MetadataCatalogue\dashboard_code\metadata-catalogue-dashboard\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EFF9CC1-152A-4BB1-9778-74719C8C9BB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{278DCF42-2545-4941-84AD-5871F869AECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6E15B39E-F836-4E17-87F3-3087AF82566E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6E15B39E-F836-4E17-87F3-3087AF82566E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -625,7 +625,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
- added a summary tab in the homepage - made accessibility improvements
</commit_message>
<xml_diff>
--- a/www/definitions.xlsx
+++ b/www/definitions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\stats\cl-out\MetadataCatalogue\dashboard_code\metadata-catalogue-dashboard\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{278DCF42-2545-4941-84AD-5871F869AECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5523630-5F23-438C-AFE3-CF40A9BDEC50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6E15B39E-F836-4E17-87F3-3087AF82566E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="72">
   <si>
     <t>Definition</t>
   </si>
@@ -98,9 +98,6 @@
     <t>Whether the item is a dashboard, a statistical report, or an indicator.</t>
   </si>
   <si>
-    <t>Tags on each item which aid filtering of types of item.</t>
-  </si>
-  <si>
     <t>A description of the item.</t>
   </si>
   <si>
@@ -222,6 +219,39 @@
   </si>
   <si>
     <t>Health &amp; Care: Acute &amp; Emergency Services| Justice Crime &amp; Violence| Early Years &amp; Young People| Alcohol : Drugs : Smoking| Health &amp; Care: Primary Community &amp; Social Care| Education| Long Term Conditions &amp; Diseases| Place &amp; physical environment| Dental Health| Housing| Income &amp; Poverty| GCR Indicators| Mental health &amp; Wellbeing|  Communicable diseases| Physical Activity| Transport| Vulnerable Populations| Diet &amp; Nutrition| Employment| Vaccinations| Place &amp; Physical Environment|  Climate &amp; Environment|  Gambling| Children &amp; Young People| Tobacco</t>
+  </si>
+  <si>
+    <t>Tags on each item which aid filtering of types of item. These can be used to search for a specific area of interesst within a health &amp; wellbeing topic.</t>
+  </si>
+  <si>
+    <t>No| Yes</t>
+  </si>
+  <si>
+    <t>Public Health Scotland (various e-mail addresses provided)| Scottish Government| ScotPHO| Improvement Service| Scottish Prison Service| Office for National Statistics| Health and Safety Executive| UK Government| Higher Education Student Statistics UK| Skills Development Scotland| Trussell Trust</t>
+  </si>
+  <si>
+    <t>Free-text instructions provided</t>
+  </si>
+  <si>
+    <t>Multiple free-text responses</t>
+  </si>
+  <si>
+    <t>Multiple permutations provided in calendar year, financial year or combined years.</t>
+  </si>
+  <si>
+    <t>Multiple dates provided in YYYY-MM-DD format (e.g, 2022-05-31), Season-Year format (e.g., Summer-2024), or Month-Year format (e.g., August-2023)</t>
+  </si>
+  <si>
+    <t>Multiple dates provided in YYYY-MM-DD format (e.g, 2024-08-31), Season-Year format  (e.g, Summer-2024), or Month-Year format (e.g., August-2024)</t>
+  </si>
+  <si>
+    <t>Multiple unique links provided</t>
+  </si>
+  <si>
+    <t>Multiple data sources provided</t>
+  </si>
+  <si>
+    <t>Various combinations of all ages ("All"), an age band (e.g., "0-4"), under a certain age (e.g., "&lt;5") or over a certain age (e.g., "65+").</t>
   </si>
 </sst>
 </file>
@@ -625,307 +655,343 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="60.5703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="71.140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="21.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.81640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="60.54296875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="71.1796875" style="2" customWidth="1"/>
     <col min="6" max="6" width="80" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="D2" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="108.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="109" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="108.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="109" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="C8" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="116" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>33</v>
+      <c r="D20" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="F20" s="2"/>
     </row>

</xml_diff>